<commit_message>
change proto stream local remote seperate
</commit_message>
<xml_diff>
--- a/tools/xlsx2xml/xlsx/Localization.xlsx
+++ b/tools/xlsx2xml/xlsx/Localization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
   <si>
     <t>Key</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>LS_LoginSuccess</t>
+    <t>LS_Info_LoginSuccess</t>
   </si>
   <si>
     <t>登录成功</t>
@@ -37,7 +37,10 @@
     <t>Login Success</t>
   </si>
   <si>
-    <t>LS_Login_Incorrect_User_Password</t>
+    <t>LocalServer</t>
+  </si>
+  <si>
+    <t>LS_Info_Login_Incorrect_User_Password</t>
   </si>
   <si>
     <t>密码错误</t>
@@ -46,7 +49,7 @@
     <t>Login Incorrect User or Password</t>
   </si>
   <si>
-    <t>LS_Heartbeat_Timeout</t>
+    <t>LS_Err_Heartbeat_Timeout</t>
   </si>
   <si>
     <t>TCP连接超时</t>
@@ -55,7 +58,16 @@
     <t>Tcp Connection Timeout</t>
   </si>
   <si>
-    <t>SRS_Start_Local_Audio</t>
+    <t>LS_Err_NoStreamRelayService_Connected</t>
+  </si>
+  <si>
+    <t>没有正在运行的流服务</t>
+  </si>
+  <si>
+    <t>No StreamRelay Service Working</t>
+  </si>
+  <si>
+    <t>SRS_Info_Start_Local_Audio</t>
   </si>
   <si>
     <t>局域网对讲开始</t>
@@ -64,7 +76,10 @@
     <t>Local Audio Start</t>
   </si>
   <si>
-    <t>SRS_Stop_Local_Audio</t>
+    <t>StreamRelay Service</t>
+  </si>
+  <si>
+    <t>SRS_Info_Stop_Local_Audio</t>
   </si>
   <si>
     <t>局域网对讲结束</t>
@@ -78,10 +93,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -93,6 +108,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -100,52 +122,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,38 +152,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,23 +182,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -235,6 +219,37 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -245,187 +260,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,32 +457,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,7 +497,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,6 +509,30 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,10 +559,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -556,133 +571,133 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1009,15 +1024,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="33.125" customWidth="1"/>
+    <col min="1" max="1" width="39.875" customWidth="1"/>
     <col min="2" max="2" width="22.875" customWidth="1"/>
     <col min="3" max="3" width="33.25" customWidth="1"/>
     <col min="4" max="4" width="23.625" customWidth="1"/>
@@ -1037,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1046,50 +1061,67 @@
       </c>
       <c r="C2" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>